<commit_message>
inputan untuk user draft
</commit_message>
<xml_diff>
--- a/File dari Pak Eflan/PERCOBAAN PROGRAM PPIC.xlsx
+++ b/File dari Pak Eflan/PERCOBAAN PROGRAM PPIC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Project Magang\ProjectMagang\File dari Pak Eflan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Magang\ProjectMagang\File dari Pak Eflan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9908F49-5807-4F7C-BEE5-15922EE8BC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E227F5-D143-40A8-BBEE-17F936D7998D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" HASIL KESELURUHAN" sheetId="1" r:id="rId1"/>
@@ -900,8 +900,8 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1376,7 +1376,9 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1533,7 +1535,7 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A2" sqref="A2:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>